<commit_message>
Ajout commissaires / membres CO connus
</commit_message>
<xml_diff>
--- a/excel/staff.xlsx
+++ b/excel/staff.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2024/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7858AD3C-4672-A746-9CCE-5C767AF9CC58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AB9C234-193E-DF45-BC77-BE6ADD48D659}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41380" yWindow="2820" windowWidth="33480" windowHeight="20380" xr2:uid="{FD29B0F2-1663-8540-80A1-3F866C889E60}"/>
+    <workbookView xWindow="33380" yWindow="6340" windowWidth="33480" windowHeight="20380" activeTab="2" xr2:uid="{FD29B0F2-1663-8540-80A1-3F866C889E60}"/>
   </bookViews>
   <sheets>
     <sheet name="CO" sheetId="1" r:id="rId1"/>
@@ -38,8 +38,26 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={BB4C3E5E-59F5-434C-B266-8F98498F7305}</author>
+  </authors>
+  <commentList>
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{BB4C3E5E-59F5-434C-B266-8F98498F7305}">
+      <text>
+        <t>[Commentaire lié à un fil de discussion]
+Votre version d’Excel vous permet de lire ce commentaire lié à un fil de discussion. Toutefois, les modifications qui y sont apportées seront supprimées si le fichier est ouvert dans une version plus récente d’Excel. En savoir plus : https://go.microsoft.com/fwlink/?linkid=870924
+Commentaire :
+    https://cc.commgr.ca/ComMgr/AssignmentsPublic/</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="108">
   <si>
     <t>noms</t>
   </si>
@@ -140,9 +158,6 @@
     <t>Facilities and logistics</t>
   </si>
   <si>
-    <t>City of Amos Representative</t>
-  </si>
-  <si>
     <t>Comité Écoresponsable</t>
   </si>
   <si>
@@ -287,15 +302,6 @@
     <t>Alica Fontaine-Fortin</t>
   </si>
   <si>
-    <t>Temple de la Renommée</t>
-  </si>
-  <si>
-    <t>Hall of Fame</t>
-  </si>
-  <si>
-    <t>Représentant de la Ville de Amos</t>
-  </si>
-  <si>
     <t>Bobby Noury</t>
   </si>
   <si>
@@ -320,14 +326,65 @@
     <t>TBD</t>
   </si>
   <si>
-    <t>TBD&lt;br/&gt;
+    <t>Kurt Sauer</t>
+  </si>
+  <si>
+    <t>Amélie Gélinas</t>
+  </si>
+  <si>
+    <t>\(819) 727-6333</t>
+  </si>
+  <si>
+    <t>Antoine St-Jean</t>
+  </si>
+  <si>
+    <t>Claudette Aylwin</t>
+  </si>
+  <si>
+    <t>Sophie-Kristine Richard</t>
+  </si>
+  <si>
+    <t>Marie-Ève Dionne&lt;br/&gt;Tina Aubé</t>
+  </si>
+  <si>
+    <t>Julie Pelletier</t>
+  </si>
+  <si>
+    <t>Claude Deraps</t>
+  </si>
+  <si>
+    <t>Steve Roussil&lt;br/&gt;Caroline Comeau</t>
+  </si>
+  <si>
+    <t>Représentant de la Ville de Val-d'Or</t>
+  </si>
+  <si>
+    <t>City of Val-d'Or Representative</t>
+  </si>
+  <si>
+    <t>Stéphane Larose&lt;br/&gt;Marc Tremblay&lt;br/&gt;Stéphane Fiset&lt;br/&gt;Francis Fortin</t>
+  </si>
+  <si>
+    <t>Michel Laverdure</t>
+  </si>
+  <si>
+    <t>Luc Lavoie</t>
+  </si>
+  <si>
+    <t>Pierre Dupuis</t>
+  </si>
+  <si>
+    <t>Vallérie Trottier</t>
+  </si>
+  <si>
+    <t>Nancy Daigle&lt;br/&gt;
 TBD</t>
   </si>
   <si>
-    <t>TBD&lt;br/&gt;
-TBD&lt;br/&gt;
-TBD&lt;br/&gt;
-TBD&lt;br/&gt;
+    <t>Steve Head&lt;br/&gt;
+Hélène Soulard&lt;br/&gt;
+Vallérie Trottier&lt;br/&gt;
+Nancy Daigle&lt;br/&gt;
 TBD&lt;br/&gt;
 TBD</t>
   </si>
@@ -336,7 +393,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -384,6 +441,12 @@
       <name val="Trebuchet MS"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -405,7 +468,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -436,9 +499,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,10 +516,16 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Gauthier Bruno" id="{F43BA70A-D507-7C4A-BCA3-F7638A62AF19}" userId="S::gauthier.bruno.2@univ.teluq.ca::aaa787f6-417e-4e71-98ea-7c31130d20cf" providerId="AD"/>
+</personList>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office 2013 – 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -497,7 +563,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -603,7 +669,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -745,18 +811,26 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
+</file>
+
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="C1" dT="2024-03-18T18:43:04.45" personId="{F43BA70A-D507-7C4A-BCA3-F7638A62AF19}" id="{BB4C3E5E-59F5-434C-B266-8F98498F7305}">
+    <text>https://cc.commgr.ca/ComMgr/AssignmentsPublic/</text>
+  </threadedComment>
+</ThreadedComments>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72262817-9D66-6D48-97C4-5126E8F8BB18}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -769,10 +843,10 @@
   <sheetData>
     <row r="1" spans="1:4" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>61</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>0</v>
@@ -783,35 +857,35 @@
     </row>
     <row r="2" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>3</v>
@@ -820,7 +894,7 @@
         <v>4</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -831,38 +905,38 @@
         <v>5</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>92</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -873,10 +947,10 @@
         <v>8</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -887,10 +961,10 @@
         <v>10</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -901,10 +975,10 @@
         <v>12</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -915,10 +989,10 @@
         <v>14</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -926,13 +1000,13 @@
         <v>16</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -943,10 +1017,10 @@
         <v>17</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -957,10 +1031,10 @@
         <v>19</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -974,7 +1048,7 @@
         <v>22</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -985,10 +1059,10 @@
         <v>23</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -999,10 +1073,10 @@
         <v>25</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1013,10 +1087,10 @@
         <v>27</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1027,10 +1101,10 @@
         <v>29</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1041,66 +1115,66 @@
         <v>31</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>33</v>
+        <v>100</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>84</v>
+        <v>99</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="17" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="C24" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1111,10 +1185,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70C23D3F-FE64-A34F-B126-68B68B58113C}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="25.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1126,10 +1200,10 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>61</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>0</v>
@@ -1137,150 +1211,139 @@
     </row>
     <row r="2" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>92</v>
+        <v>42</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>92</v>
+        <v>43</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="34" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>92</v>
+        <v>83</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>92</v>
+      <c r="C5" s="5" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>92</v>
+      <c r="C6" s="5" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>92</v>
+        <v>49</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>92</v>
+        <v>39</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>83</v>
+      <c r="A9" s="7" t="s">
+        <v>51</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>92</v>
+        <v>51</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>92</v>
+        <v>41</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>92</v>
+        <v>52</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>92</v>
+      <c r="C12" s="5" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C13" s="12" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B15" s="6"/>
-      <c r="C15" s="5"/>
+      <c r="C13" s="5" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B14" s="6"/>
+      <c r="C14" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1289,11 +1352,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{823BAD0D-314A-CF4D-A7B3-D837A1000984}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{823BAD0D-314A-CF4D-A7B3-D837A1000984}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1305,10 +1368,10 @@
   <sheetData>
     <row r="1" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>61</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>0</v>
@@ -1316,39 +1379,40 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="102" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>94</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="10" t="s">
-        <v>64</v>
-      </c>
       <c r="C4" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1357,7 +1421,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1369,10 +1433,10 @@
   <sheetData>
     <row r="1" spans="1:3" s="7" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>61</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>0</v>
@@ -1380,32 +1444,32 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C2" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" s="10" t="s">
         <v>63</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>64</v>
       </c>
       <c r="C4" t="str">
         <f>COMM!C4</f>

</xml_diff>

<commit_message>
MAJ liste staff / CO
</commit_message>
<xml_diff>
--- a/excel/staff.xlsx
+++ b/excel/staff.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2024/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F209773A-0082-8E4B-8B45-462ED8057761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{213B631F-56CA-E549-A6DA-7C8D101EA3A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33380" yWindow="6340" windowWidth="33480" windowHeight="20380" xr2:uid="{FD29B0F2-1663-8540-80A1-3F866C889E60}"/>
+    <workbookView xWindow="16820" yWindow="560" windowWidth="16720" windowHeight="20380" xr2:uid="{FD29B0F2-1663-8540-80A1-3F866C889E60}"/>
   </bookViews>
   <sheets>
     <sheet name="CO" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="120">
   <si>
     <t>noms</t>
   </si>
@@ -302,9 +302,6 @@
     <t>Alica Fontaine-Fortin</t>
   </si>
   <si>
-    <t>Bobby Noury</t>
-  </si>
-  <si>
     <t>\(819) 856-6821</t>
   </si>
   <si>
@@ -369,9 +366,6 @@
   </si>
   <si>
     <t>Luc Lavoie</t>
-  </si>
-  <si>
-    <t>Pierre Dupuis</t>
   </si>
   <si>
     <t>Vallérie Trottier</t>
@@ -393,6 +387,42 @@
   </si>
   <si>
     <t>Baroudeur Support Technique&lt;br/&gt;Matis Boyer</t>
+  </si>
+  <si>
+    <t>\(819) 744-7765</t>
+  </si>
+  <si>
+    <t>\(819) 856-0772</t>
+  </si>
+  <si>
+    <t>\(418) 690-6564</t>
+  </si>
+  <si>
+    <t>Équipe Subway&lt;br/&gt;Mathieu Roy</t>
+  </si>
+  <si>
+    <t>\(819) 444-9746</t>
+  </si>
+  <si>
+    <t>\(819) 860-8614&lt;br/&gt;(819) 860-9605</t>
+  </si>
+  <si>
+    <t>\(819) 856-6200</t>
+  </si>
+  <si>
+    <t>\(819) 856-8665</t>
+  </si>
+  <si>
+    <t>\(819 825-2210&lt;br/&gt;(819) 860-1580</t>
+  </si>
+  <si>
+    <t>Robert Noury</t>
+  </si>
+  <si>
+    <t>\(819) 856-1565</t>
+  </si>
+  <si>
+    <t>\(819) 856-5375</t>
   </si>
 </sst>
 </file>
@@ -830,7 +860,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -874,7 +904,7 @@
         <v>36</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>77</v>
@@ -919,10 +949,10 @@
         <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="34" x14ac:dyDescent="0.2">
@@ -930,13 +960,13 @@
         <v>74</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -947,10 +977,10 @@
         <v>8</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>88</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="22" customHeight="1" x14ac:dyDescent="0.2">
@@ -961,10 +991,10 @@
         <v>10</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -975,10 +1005,10 @@
         <v>12</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>104</v>
+        <v>87</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -989,10 +1019,10 @@
         <v>14</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>88</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1017,10 +1047,10 @@
         <v>17</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>88</v>
+        <v>111</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>88</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -1031,10 +1061,10 @@
         <v>19</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>88</v>
+        <v>113</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -1059,10 +1089,10 @@
         <v>23</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>88</v>
+        <v>114</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -1073,10 +1103,10 @@
         <v>25</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>88</v>
+        <v>115</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1087,10 +1117,10 @@
         <v>27</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>88</v>
+        <v>116</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1101,10 +1131,10 @@
         <v>29</v>
       </c>
       <c r="C19" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1115,24 +1145,24 @@
         <v>31</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>88</v>
+        <v>118</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>88</v>
+        <v>119</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1143,24 +1173,24 @@
         <v>33</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="34" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">
@@ -1217,7 +1247,7 @@
         <v>42</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -1228,7 +1258,7 @@
         <v>43</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="34" customHeight="1" x14ac:dyDescent="0.2">
@@ -1236,10 +1266,10 @@
         <v>44</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1250,7 +1280,7 @@
         <v>46</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1261,7 +1291,7 @@
         <v>48</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1272,7 +1302,7 @@
         <v>49</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1283,7 +1313,7 @@
         <v>39</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1294,7 +1324,7 @@
         <v>51</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1305,7 +1335,7 @@
         <v>41</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1316,7 +1346,7 @@
         <v>52</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1327,7 +1357,7 @@
         <v>54</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="17" x14ac:dyDescent="0.2">
@@ -1338,7 +1368,7 @@
         <v>56</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -1385,7 +1415,7 @@
         <v>72</v>
       </c>
       <c r="C2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="102" x14ac:dyDescent="0.2">
@@ -1396,7 +1426,7 @@
         <v>61</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1407,7 +1437,7 @@
         <v>63</v>
       </c>
       <c r="C4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -1450,7 +1480,7 @@
         <v>72</v>
       </c>
       <c r="C2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="34" x14ac:dyDescent="0.2">
@@ -1461,7 +1491,7 @@
         <v>61</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Ajout téléphone Stéphane Larose
</commit_message>
<xml_diff>
--- a/excel/staff.xlsx
+++ b/excel/staff.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2024/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{213B631F-56CA-E549-A6DA-7C8D101EA3A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CE24760-ABC5-DB4B-8D0A-31E4FAB38618}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16820" yWindow="560" windowWidth="16720" windowHeight="20380" xr2:uid="{FD29B0F2-1663-8540-80A1-3F866C889E60}"/>
+    <workbookView xWindow="16820" yWindow="560" windowWidth="37180" windowHeight="23720" xr2:uid="{FD29B0F2-1663-8540-80A1-3F866C889E60}"/>
   </bookViews>
   <sheets>
     <sheet name="CO" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="121">
   <si>
     <t>noms</t>
   </si>
@@ -423,6 +423,9 @@
   </si>
   <si>
     <t>\(819) 856-5375</t>
+  </si>
+  <si>
+    <t>\(819) 856-1565&lt;br/&gt;TBD&lt;br/&gt;TBD&lt;br/&gt;TBD</t>
   </si>
 </sst>
 </file>
@@ -860,7 +863,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1190,7 +1193,7 @@
         <v>100</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>87</v>
+        <v>120</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="17" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Ajout responsable centrale - staff
</commit_message>
<xml_diff>
--- a/excel/staff.xlsx
+++ b/excel/staff.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2024/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CE24760-ABC5-DB4B-8D0A-31E4FAB38618}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FECB76B-1EB4-6146-BD66-83F1F732C4F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16820" yWindow="560" windowWidth="37180" windowHeight="23720" xr2:uid="{FD29B0F2-1663-8540-80A1-3F866C889E60}"/>
+    <workbookView xWindow="36620" yWindow="1460" windowWidth="37180" windowHeight="23720" xr2:uid="{FD29B0F2-1663-8540-80A1-3F866C889E60}"/>
   </bookViews>
   <sheets>
     <sheet name="CO" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="122">
   <si>
     <t>noms</t>
   </si>
@@ -426,6 +426,9 @@
   </si>
   <si>
     <t>\(819) 856-1565&lt;br/&gt;TBD&lt;br/&gt;TBD&lt;br/&gt;TBD</t>
+  </si>
+  <si>
+    <t>Emmanuel Gilbert</t>
   </si>
 </sst>
 </file>
@@ -863,7 +866,7 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1008,7 +1011,7 @@
         <v>12</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>87</v>
+        <v>121</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>87</v>

</xml_diff>

<commit_message>
AJout commissaire Johanne Binet
</commit_message>
<xml_diff>
--- a/excel/staff.xlsx
+++ b/excel/staff.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brunogauthier/Documents/guide2024/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A584E281-D355-0B4E-ABBA-822C11F5CAD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{380C61BE-AB52-094F-AADC-E1FFA71E0A11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32580" yWindow="3020" windowWidth="33600" windowHeight="20500" activeTab="2" xr2:uid="{FD29B0F2-1663-8540-80A1-3F866C889E60}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" activeTab="2" xr2:uid="{FD29B0F2-1663-8540-80A1-3F866C889E60}"/>
   </bookViews>
   <sheets>
     <sheet name="CO" sheetId="1" r:id="rId1"/>
@@ -458,7 +458,7 @@
   <si>
     <t>Steve Head&lt;br/&gt;
 Andrew Paradowski&lt;br/&gt;
-TBD&lt;br/&gt;
+Johanne Binet&lt;br/&gt;
 Nancy Daigle&lt;br/&gt;
 Félix-Antoine Malo&lt;br/&gt;
 Geneviève Marcotte</t>
@@ -1417,7 +1417,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>